<commit_message>
feat(biomethane): fix doublon name in xlsx file
</commit_message>
<xml_diff>
--- a/web/feedstocks/fixtures/import-intrants-biomethane.xlsx
+++ b/web/feedstocks/fixtures/import-intrants-biomethane.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yohann/Documents/Projets/YomiCode/CarbuRe/carbure/web/feedstocks/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDF6005-14EA-5C4C-8262-D2A5714296D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30AFABC-8681-4A45-B6FF-F0BF1FD25DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="1420" windowWidth="26820" windowHeight="16160" xr2:uid="{CED13A77-16D8-5E4B-B1C7-A722F681FD6F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CED13A77-16D8-5E4B-B1C7-A722F681FD6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Classifications" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="213">
   <si>
     <t>Residues</t>
   </si>
@@ -113,6 +113,9 @@
     <t>Orge</t>
   </si>
   <si>
+    <t>Mais - CIVE</t>
+  </si>
+  <si>
     <t>Biomasse agricole - Non alimentaire</t>
   </si>
   <si>
@@ -221,30 +224,12 @@
     <t>Autres déchets de STEP urbaine</t>
   </si>
   <si>
-    <t>Graisses d'abattoir</t>
-  </si>
-  <si>
     <t>Autres déchets d’abattoir (résidus animaux (non gras) Catégorie 1)</t>
   </si>
   <si>
-    <t>Matières stercoraires</t>
-  </si>
-  <si>
-    <t>Boues de STEP d'abattoir</t>
-  </si>
-  <si>
-    <t>Autres déchets d'abattoirs</t>
-  </si>
-  <si>
     <t>Déchets de poissons et de fruits de mer</t>
   </si>
   <si>
-    <t>Déchets de viandes</t>
-  </si>
-  <si>
-    <t>Produits carnés non consommés/invendus</t>
-  </si>
-  <si>
     <t>Industriel</t>
   </si>
   <si>
@@ -257,21 +242,6 @@
     <t>Graisses de flottation issues du traitement des eaux usées</t>
   </si>
   <si>
-    <t>Autres déchets animaux issus d'IAA</t>
-  </si>
-  <si>
-    <t>Déchets de la préparation de produits laitier et produits laitier non consommés/invendus… (lactoserum, Lait, fromage, caséïne…)</t>
-  </si>
-  <si>
-    <t>Graisses de flottation d’IAA de produits laitiers</t>
-  </si>
-  <si>
-    <t>Boues de STEP de l’IAA de produits laitiers</t>
-  </si>
-  <si>
-    <t>Autres déchets d’IAA de produits laitiers</t>
-  </si>
-  <si>
     <t>Co-produit</t>
   </si>
   <si>
@@ -281,6 +251,9 @@
     <t>Industrie agroalimentaire</t>
   </si>
   <si>
+    <t>Glycérine animale</t>
+  </si>
+  <si>
     <t>Glycérine végétale</t>
   </si>
   <si>
@@ -293,24 +266,12 @@
     <t>Autres</t>
   </si>
   <si>
-    <t>Glycérine</t>
-  </si>
-  <si>
-    <t>Déclassement et déchets de fruits/légumes/tubercules/condiment</t>
-  </si>
-  <si>
     <t>Pulpes de betteraves/radidelles/herbes pressées</t>
   </si>
   <si>
     <t>Mélasse</t>
   </si>
   <si>
-    <t>Drêches et vinasse de lies de vin</t>
-  </si>
-  <si>
-    <t>Déchets de céréales et oléoprotéagineux (séchage, stockage, tri…)</t>
-  </si>
-  <si>
     <t>Déchets de la préparation de produits végétaux et produits végétaux non consommés/invendus (pain, pâtes, barres céréales, confiseries…)</t>
   </si>
   <si>
@@ -476,12 +437,6 @@
     <t>Herbe - Praires temporaires</t>
   </si>
   <si>
-    <t>Résidus de grandes cultures</t>
-  </si>
-  <si>
-    <t>Autres résidus</t>
-  </si>
-  <si>
     <t>Refus de silo d’ensilage</t>
   </si>
   <si>
@@ -500,12 +455,6 @@
     <t>Huiles alimentaires usagées d'origine non-spécifiée</t>
   </si>
   <si>
-    <t>Huiles et matières grasses (avec produits animaux)</t>
-  </si>
-  <si>
-    <t>Glycérine animale issue de graisse d'équarrissage</t>
-  </si>
-  <si>
     <t>Marc de raisin</t>
   </si>
   <si>
@@ -576,6 +525,156 @@
   </si>
   <si>
     <t>is_methanizable</t>
+  </si>
+  <si>
+    <t>Colza - CIVE</t>
+  </si>
+  <si>
+    <t>Sorgho - CIVE</t>
+  </si>
+  <si>
+    <t>Triticale - CIVE</t>
+  </si>
+  <si>
+    <t>Seigle - CIVE</t>
+  </si>
+  <si>
+    <t>Orge - CIVE</t>
+  </si>
+  <si>
+    <t>Autres cultures - CIVE</t>
+  </si>
+  <si>
+    <t>Résidus de cultures</t>
+  </si>
+  <si>
+    <t>Autres résidus de champs / récolte</t>
+  </si>
+  <si>
+    <t>Graisses d'abattoir (Cat 1)</t>
+  </si>
+  <si>
+    <t>Graisses d'abattoir (Cat 2)</t>
+  </si>
+  <si>
+    <t>Graisses d'abattoir (Cat 3)</t>
+  </si>
+  <si>
+    <t>Matières stercoraires (Cat 1)</t>
+  </si>
+  <si>
+    <t>Matières stercoraires (Cat 2)</t>
+  </si>
+  <si>
+    <t>Matières stercoraires (Cat 3)</t>
+  </si>
+  <si>
+    <t>Boues de STEP d'abattoir (Cat 1)</t>
+  </si>
+  <si>
+    <t>Autres déchets d'abattoirs (Cat 1)</t>
+  </si>
+  <si>
+    <t>Autres déchets d'abattoirs (Cat 2)</t>
+  </si>
+  <si>
+    <t>Autres déchets d'abattoirs (Cat 3)</t>
+  </si>
+  <si>
+    <t>Déchets de viandes (Cat 1)</t>
+  </si>
+  <si>
+    <t>Déchets de viandes (Cat 2)</t>
+  </si>
+  <si>
+    <t>Déchets de viandes (Cat 3)</t>
+  </si>
+  <si>
+    <t>Huiles et matières grasses (avec produits animaux) (Cat 1)</t>
+  </si>
+  <si>
+    <t>Huiles et matières grasses (avec produits animaux) (Cat 2)</t>
+  </si>
+  <si>
+    <t>Huiles et matières grasses (avec produits animaux) (Cat 3)</t>
+  </si>
+  <si>
+    <t>Produits carnés non consommés/invendus (Cat 1)</t>
+  </si>
+  <si>
+    <t>Produits carnés non consommés/invendus (Cat 2)</t>
+  </si>
+  <si>
+    <t>Produits carnés non consommés/invendus (Cat 3)</t>
+  </si>
+  <si>
+    <t>Autres déchets animaux issus d'IAA (Cat 1)</t>
+  </si>
+  <si>
+    <t>Autres déchets animaux issus d'IAA (Cat 2)</t>
+  </si>
+  <si>
+    <t>Autres déchets animaux issus d'IAA (Cat 3)</t>
+  </si>
+  <si>
+    <t>Déchets de la préparation de produits laitier et produits laitier non consommés/invendus… (lactoserum, Lait, fromage, caséïne…) (Cat 1)</t>
+  </si>
+  <si>
+    <t>Déchets de la préparation de produits laitier et produits laitier non consommés/invendus… (lactoserum, Lait, fromage, caséïne…) (Cat 2)</t>
+  </si>
+  <si>
+    <t>Déchets de la préparation de produits laitier et produits laitier non consommés/invendus… (lactoserum, Lait, fromage, caséïne…) (Cat 3)</t>
+  </si>
+  <si>
+    <t>Graisses de flottation d’IAA de produits laitiers (Cat 1)</t>
+  </si>
+  <si>
+    <t>Graisses de flottation d’IAA de produits laitiers (Cat 2)</t>
+  </si>
+  <si>
+    <t>Graisses de flottation d’IAA de produits laitiers (Cat 3)</t>
+  </si>
+  <si>
+    <t>Boues de STEP de l’IAA de produits laitiers (Cat 1)</t>
+  </si>
+  <si>
+    <t>Boues de STEP de l’IAA de produits laitiers (Cat 2)</t>
+  </si>
+  <si>
+    <t>Boues de STEP de l’IAA de produits laitiers (Cat 3)</t>
+  </si>
+  <si>
+    <t>Autres déchets d’IAA de produits laitiers (Cat 1)</t>
+  </si>
+  <si>
+    <t>Autres déchets d’IAA de produits laitiers (Cat 2)</t>
+  </si>
+  <si>
+    <t>Autres déchets d’IAA de produits laitiers (Cat 3)</t>
+  </si>
+  <si>
+    <t>Autre glycérine</t>
+  </si>
+  <si>
+    <t>Déclassement de fruits/légumes/tubercules/condiment</t>
+  </si>
+  <si>
+    <t>Déchets de fruits/légumes/tubercules/condiment</t>
+  </si>
+  <si>
+    <t>Lies de vin</t>
+  </si>
+  <si>
+    <t>Déchets de céréales (séchage, stockage, tri…)</t>
+  </si>
+  <si>
+    <t>Déchets oléoprotéagineux (séchage, stockage, tri…)</t>
+  </si>
+  <si>
+    <t>Boues de STEP d'abattoir (Cat 2)</t>
+  </si>
+  <si>
+    <t>Boues de STEP d'abattoir (Cat 3)</t>
   </si>
 </sst>
 </file>
@@ -964,35 +1063,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C854CE-F7D6-9346-B585-BC5C70CEEDF8}">
   <dimension ref="A1:F1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="B53" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="53.83203125" customWidth="1"/>
-    <col min="3" max="3" width="52" customWidth="1"/>
-    <col min="4" max="4" width="93.6640625" customWidth="1"/>
+    <col min="2" max="2" width="73.33203125" customWidth="1"/>
+    <col min="3" max="3" width="56.83203125" customWidth="1"/>
+    <col min="4" max="4" width="112.33203125" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="6" max="6" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -1010,7 +1109,7 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1027,7 +1126,7 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1044,7 +1143,7 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1061,7 +1160,7 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1078,7 +1177,7 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1095,7 +1194,7 @@
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1112,7 +1211,7 @@
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1129,7 +1228,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1146,7 +1245,7 @@
         <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1163,7 +1262,7 @@
         <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1180,7 +1279,7 @@
         <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1197,7 +1296,7 @@
         <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1205,7 +1304,7 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
@@ -1214,7 +1313,7 @@
         <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1222,7 +1321,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
@@ -1231,7 +1330,7 @@
         <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1239,16 +1338,16 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="E16" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1256,16 +1355,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="E17" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1273,16 +1372,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
         <v>19</v>
       </c>
       <c r="D18" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="E18" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1290,16 +1389,16 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C19" t="s">
         <v>19</v>
       </c>
       <c r="D19" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="E19" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1307,7 +1406,7 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
@@ -1316,7 +1415,7 @@
         <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1324,7 +1423,7 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
@@ -1333,7 +1432,7 @@
         <v>22</v>
       </c>
       <c r="E21" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1341,7 +1440,7 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
@@ -1350,7 +1449,7 @@
         <v>23</v>
       </c>
       <c r="E22" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1358,7 +1457,7 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
@@ -1367,7 +1466,7 @@
         <v>24</v>
       </c>
       <c r="E23" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1375,16 +1474,16 @@
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="E24" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1392,16 +1491,16 @@
         <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C25" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D25" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="E25" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1409,16 +1508,16 @@
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C26" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D26" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="E26" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1426,16 +1525,16 @@
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C27" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="D27" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="E27" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1443,16 +1542,16 @@
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C28" t="s">
         <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E28" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1460,16 +1559,16 @@
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C29" t="s">
         <v>19</v>
       </c>
       <c r="D29" t="s">
-        <v>20</v>
+        <v>163</v>
       </c>
       <c r="E29" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1477,16 +1576,16 @@
         <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
       </c>
       <c r="D30" t="s">
-        <v>21</v>
+        <v>164</v>
       </c>
       <c r="E30" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1494,16 +1593,16 @@
         <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C31" t="s">
         <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>22</v>
+        <v>165</v>
       </c>
       <c r="E31" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1511,16 +1610,16 @@
         <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C32" t="s">
         <v>17</v>
       </c>
       <c r="D32" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="E32" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1528,16 +1627,16 @@
         <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C33" t="s">
         <v>17</v>
       </c>
       <c r="D33" t="s">
-        <v>24</v>
+        <v>167</v>
       </c>
       <c r="E33" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1545,16 +1644,16 @@
         <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C34" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="D34" t="s">
-        <v>110</v>
+        <v>168</v>
       </c>
       <c r="E34" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1562,16 +1661,16 @@
         <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C35" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D35" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="E35" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1579,16 +1678,16 @@
         <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C36" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D36" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="E36" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1596,16 +1695,16 @@
         <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C37" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D37" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="E37" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1613,33 +1712,33 @@
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C38" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D38" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="E38" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B39" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D39" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E39" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1650,13 +1749,13 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D40" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E40" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1667,13 +1766,13 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D41" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E41" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1684,13 +1783,13 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D42" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="E42" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1701,1484 +1800,1484 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D43" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="E43" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B44" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C44" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D44" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="E44" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B45" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C45" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D45" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="E45" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B46" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C46" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D46" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E46" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B47" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C47" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D47" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E47" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C48" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D48" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E48" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B49" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C49" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D49" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E49" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B50" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C50" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D50" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E50" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B51" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C51" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D51" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E51" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B52" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C52" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D52" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E52" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B53" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C53" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D53" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E53" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B54" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C54" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D54" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E54" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B55" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C55" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D55" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E55" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B56" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C56" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D56" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E56" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B57" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C57" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D57" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="E57" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B58" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C58" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D58" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="E58" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B59" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C59" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D59" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="E59" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B60" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C60" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D60" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="E60" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B61" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C61" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D61" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E61" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B62" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C62" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D62" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E62" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C63" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D63" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E63" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B64" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C64" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D64" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E64" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B65" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C65" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D65" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E65" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B66" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="D66" t="s">
-        <v>61</v>
+        <v>171</v>
       </c>
       <c r="E66" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B67" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="D67" t="s">
-        <v>61</v>
+        <v>172</v>
       </c>
       <c r="E67" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B68" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="D68" t="s">
-        <v>61</v>
+        <v>173</v>
       </c>
       <c r="E68" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B69" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C69" t="s">
         <v>62</v>
       </c>
       <c r="D69" t="s">
-        <v>63</v>
+        <v>174</v>
       </c>
       <c r="E69" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B70" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C70" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="D70" t="s">
-        <v>63</v>
+        <v>175</v>
       </c>
       <c r="E70" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B71" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="C71" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D71" t="s">
-        <v>63</v>
+        <v>176</v>
       </c>
       <c r="E71" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B72" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C72" t="s">
         <v>62</v>
       </c>
       <c r="D72" t="s">
-        <v>64</v>
+        <v>177</v>
       </c>
       <c r="E72" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B73" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C73" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="D73" t="s">
-        <v>64</v>
+        <v>211</v>
       </c>
       <c r="E73" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B74" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="C74" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D74" t="s">
-        <v>64</v>
+        <v>212</v>
       </c>
       <c r="E74" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B75" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C75" t="s">
         <v>62</v>
       </c>
       <c r="D75" t="s">
-        <v>65</v>
+        <v>178</v>
       </c>
       <c r="E75" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B76" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C76" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="D76" t="s">
-        <v>65</v>
+        <v>179</v>
       </c>
       <c r="E76" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B77" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="C77" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D77" t="s">
-        <v>65</v>
+        <v>180</v>
       </c>
       <c r="E77" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B78" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C78" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D78" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E78" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B79" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D79" t="s">
-        <v>67</v>
+        <v>181</v>
       </c>
       <c r="E79" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B80" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="D80" t="s">
-        <v>67</v>
+        <v>182</v>
       </c>
       <c r="E80" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B81" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="D81" t="s">
-        <v>67</v>
+        <v>183</v>
       </c>
       <c r="E81" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B82" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D82" t="s">
-        <v>154</v>
+        <v>184</v>
       </c>
       <c r="E82" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B83" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="D83" t="s">
-        <v>154</v>
+        <v>185</v>
       </c>
       <c r="E83" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B84" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="D84" t="s">
-        <v>154</v>
+        <v>186</v>
       </c>
       <c r="E84" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B85" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D85" t="s">
-        <v>68</v>
+        <v>187</v>
       </c>
       <c r="E85" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B86" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="D86" t="s">
-        <v>68</v>
+        <v>188</v>
       </c>
       <c r="E86" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B87" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="D87" t="s">
-        <v>68</v>
+        <v>189</v>
       </c>
       <c r="E87" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B88" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D88" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E88" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B89" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C89" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D89" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E89" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B90" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D90" t="s">
-        <v>73</v>
+        <v>190</v>
       </c>
       <c r="E90" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B91" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="D91" t="s">
-        <v>73</v>
+        <v>191</v>
       </c>
       <c r="E91" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B92" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="D92" t="s">
-        <v>73</v>
+        <v>192</v>
       </c>
       <c r="E92" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B93" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D93" t="s">
-        <v>74</v>
+        <v>193</v>
       </c>
       <c r="E93" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B94" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="D94" t="s">
-        <v>74</v>
+        <v>194</v>
       </c>
       <c r="E94" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B95" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="D95" t="s">
-        <v>74</v>
+        <v>195</v>
       </c>
       <c r="E95" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B96" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="D96" t="s">
-        <v>75</v>
+        <v>196</v>
       </c>
       <c r="E96" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B97" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="D97" t="s">
-        <v>75</v>
+        <v>197</v>
       </c>
       <c r="E97" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B98" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="D98" t="s">
-        <v>75</v>
+        <v>198</v>
       </c>
       <c r="E98" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B99" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D99" t="s">
-        <v>76</v>
+        <v>199</v>
       </c>
       <c r="E99" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B100" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="D100" t="s">
-        <v>76</v>
+        <v>200</v>
       </c>
       <c r="E100" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B101" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="D101" t="s">
-        <v>76</v>
+        <v>201</v>
       </c>
       <c r="E101" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B102" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D102" t="s">
-        <v>77</v>
+        <v>202</v>
       </c>
       <c r="E102" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B103" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="D103" t="s">
-        <v>77</v>
+        <v>203</v>
       </c>
       <c r="E103" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B104" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="D104" t="s">
-        <v>77</v>
+        <v>204</v>
       </c>
       <c r="E104" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B105" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C105" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D105" t="s">
-        <v>155</v>
+        <v>71</v>
       </c>
       <c r="E105" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B106" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C106" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D106" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E106" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B107" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C107" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D107" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E107" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B108" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C108" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D108" t="s">
-        <v>85</v>
+        <v>205</v>
       </c>
       <c r="E108" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B109" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C109" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D109" t="s">
-        <v>86</v>
+        <v>206</v>
       </c>
       <c r="E109" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B110" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C110" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D110" t="s">
-        <v>86</v>
+        <v>207</v>
       </c>
       <c r="E110" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B111" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C111" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D111" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="E111" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B112" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C112" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D112" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="E112" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B113" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C113" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D113" t="s">
-        <v>89</v>
+        <v>208</v>
       </c>
       <c r="E113" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B114" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C114" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D114" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="E114" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B115" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C115" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D115" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="E115" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B116" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C116" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D116" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="E116" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B117" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C117" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D117" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="E117" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B118" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C118" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D118" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="E118" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B119" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C119" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D119" t="s">
-        <v>90</v>
+        <v>209</v>
       </c>
       <c r="E119" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B120" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C120" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D120" t="s">
-        <v>90</v>
+        <v>210</v>
       </c>
       <c r="E120" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B121" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C121" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D121" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="E121" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B122" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C122" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D122" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="E122" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B123" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C123" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D123" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="E123" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B124" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C124" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D124" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="E124" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B125" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C125" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D125" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E125" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B126" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C126" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D126" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="E126" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B127" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C127" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D127" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E127" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B128" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C128" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D128" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="E128" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B129" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C129" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="D129" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="E129" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B130" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D130" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="E130" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B131" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C131" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D131" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="E131" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B132" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C132" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D132" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="E132" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B133" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C133" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D133" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="E133" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B134" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="D134" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="E134" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B135" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="D135" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="E135" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
@@ -3186,16 +3285,16 @@
         <v>16</v>
       </c>
       <c r="B136" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="C136" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D136" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="E136" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
@@ -3206,13 +3305,13 @@
         <v>1</v>
       </c>
       <c r="C137" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="D137" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="E137" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
@@ -3223,13 +3322,13 @@
         <v>1</v>
       </c>
       <c r="C138" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="D138" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="E138" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
@@ -3240,13 +3339,13 @@
         <v>1</v>
       </c>
       <c r="C139" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="D139" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="E139" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
@@ -3257,13 +3356,13 @@
         <v>1</v>
       </c>
       <c r="C140" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="D140" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="E140" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
@@ -3274,13 +3373,13 @@
         <v>1</v>
       </c>
       <c r="C141" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D141" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="E141" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
@@ -3291,13 +3390,13 @@
         <v>1</v>
       </c>
       <c r="C142" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="D142" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="E142" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
@@ -3308,13 +3407,13 @@
         <v>1</v>
       </c>
       <c r="C143" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="D143" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="E143" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
@@ -3325,72 +3424,72 @@
         <v>1</v>
       </c>
       <c r="C144" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="D144" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="E144" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B145" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="D145" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="E145" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B146" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C146" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="D146" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="E146" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B147" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C147" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="D147" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="E147" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D148" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="E148" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
@@ -3398,16 +3497,16 @@
         <v>0</v>
       </c>
       <c r="B149" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C149" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="D149" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="E149" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>